<commit_message>
Improved scripts by using coco_categories.json as default, updated ap_scores.xlsx with results from fixed annotation files
</commit_message>
<xml_diff>
--- a/scripts/ap_scores.xlsx
+++ b/scripts/ap_scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\University\2020\COMP7860\Repositories\comp7860-final-report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\University\2020\COMP7860\Repositories\automl\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0C2EE3-F09E-41F8-AFDE-BBB0625EED08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484639B1-E4DE-408D-859F-30925063E8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="220">
   <si>
     <t>AP</t>
   </si>
@@ -675,9 +675,6 @@
     <t>cls_loss</t>
   </si>
   <si>
-    <t>global_step</t>
-  </si>
-  <si>
     <t>loss</t>
   </si>
   <si>
@@ -688,6 +685,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1194,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1199,8 +1202,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1248,10 +1249,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="0.00000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00000000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1273,9 +1274,9 @@
     <sortCondition descending="1" ref="C1:C201"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{77FF0771-F246-447C-A669-5C8E4D8D431C}" name="ID" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{77FF0771-F246-447C-A669-5C8E4D8D431C}" name="ID" dataDxfId="1"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Class"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="AP" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="AP" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{26CC4406-809B-4507-ACF7-EEB9CF741B83}" name="Shared"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1582,14 +1583,14 @@
   <dimension ref="A1:M201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
@@ -1601,57 +1602,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" t="s">
         <v>218</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>1.1904999999999999E-4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3.9141499999999999E-3</v>
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>0.67846423</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2.0987999999999999E-4</v>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4.9148249999999997E-2</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0.39141500000000001</v>
+        <v>60</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.67846423</v>
       </c>
       <c r="M2" s="3" t="b">
         <v>1</v>
@@ -1659,57 +1660,57 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3.4280399999999998E-3</v>
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>0.59139759999999997</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1.1656E-4</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>7.0917369999999993E-2</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0.342804</v>
+        <v>35</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.59139759999999997</v>
       </c>
       <c r="M3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.1976800000000001E-3</v>
+        <v>187</v>
+      </c>
+      <c r="C4">
+        <v>0.58981185999999997</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3.0215E-4</v>
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>5.3920530000000001E-2</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="L4" s="7">
-        <v>0.319768</v>
+        <v>187</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.58981185999999997</v>
       </c>
       <c r="M4" s="3" t="b">
         <v>1</v>
@@ -1717,144 +1718,144 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.8281399999999998E-3</v>
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0.57265829999999995</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>204</v>
-      </c>
-      <c r="H5" s="1">
-        <v>7.5690000000000002E-5</v>
+        <v>203</v>
+      </c>
+      <c r="H5">
+        <v>6.1417609999999997E-2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0.28281400000000001</v>
+        <v>28</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.57265829999999995</v>
       </c>
       <c r="M5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.3479900000000001E-3</v>
+        <v>66</v>
+      </c>
+      <c r="C6">
+        <v>0.54692589999999996</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>205</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2.7750000000000002E-4</v>
+        <v>204</v>
+      </c>
+      <c r="H6">
+        <v>3.4702219999999999E-2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" s="7">
-        <v>0.134799</v>
+        <v>66</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.54692589999999996</v>
       </c>
       <c r="M6" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.3235499999999999E-3</v>
+        <v>202</v>
+      </c>
+      <c r="C7">
+        <v>0.54321870000000005</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>206</v>
-      </c>
-      <c r="H7" s="1">
-        <v>4.340223E-2</v>
+        <v>205</v>
+      </c>
+      <c r="H7">
+        <v>6.0564099999999999E-3</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0.132355</v>
+        <v>202</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.54321870000000005</v>
       </c>
       <c r="M7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.19169E-3</v>
+        <v>103</v>
+      </c>
+      <c r="C8">
+        <v>0.50333559999999999</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>207</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1.175732E-2</v>
+        <v>206</v>
+      </c>
+      <c r="H8">
+        <v>0.12487373</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="7">
-        <v>0.119169</v>
+        <v>103</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.50333559999999999</v>
       </c>
       <c r="M8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.12765E-3</v>
+        <v>126</v>
+      </c>
+      <c r="C9">
+        <v>0.47457012999999998</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1.6515519999999999E-2</v>
+        <v>207</v>
+      </c>
+      <c r="H9">
+        <v>7.90323E-2</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="8">
-        <v>0.112765</v>
+        <v>126</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.47457012999999998</v>
       </c>
       <c r="M9" s="4" t="b">
         <v>1</v>
@@ -1862,232 +1863,241 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="1">
-        <v>7.6369000000000003E-4</v>
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0.40113068000000002</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>209</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2.9835299999999999E-2</v>
+        <v>208</v>
+      </c>
+      <c r="H10">
+        <v>6.0937539999999998E-2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="7">
-        <v>7.6369000000000006E-2</v>
+        <v>4</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.40113068000000002</v>
       </c>
       <c r="M10" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="1">
-        <v>7.6256000000000002E-4</v>
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <v>0.39886070000000001</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.0358300000000001E-2</v>
+        <v>209</v>
+      </c>
+      <c r="H11">
+        <v>9.9155699999999999E-2</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.39886070000000001</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1">
-        <v>7.4465000000000002E-4</v>
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>0.37544090000000002</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>211</v>
-      </c>
-      <c r="H12" s="1">
-        <v>5.1875300000000001E-3</v>
+        <v>210</v>
+      </c>
+      <c r="H12">
+        <v>0.10270826</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="1">
-        <v>4.9850000000000003E-4</v>
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>0.36378345000000001</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>212</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.3423900000000002E-3</v>
+        <v>211</v>
+      </c>
+      <c r="H13">
+        <v>3.0311689999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3.0278999999999999E-4</v>
+        <v>116</v>
+      </c>
+      <c r="C14">
+        <v>0.35684195000000002</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>213</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1.2812355</v>
+        <v>212</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2.8656999999999999E-4</v>
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>0.34831065</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>214</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
+        <v>213</v>
+      </c>
+      <c r="H15">
+        <v>4.5277175999999999</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2.1484999999999999E-4</v>
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>0.34465677</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>215</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1.5434855999999999</v>
+        <v>214</v>
+      </c>
+      <c r="H16">
+        <v>4.6228680000000004</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1.8016000000000001E-4</v>
+        <v>157</v>
+      </c>
+      <c r="C17">
+        <v>0.34082356000000003</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1.6593000000000001E-4</v>
+        <v>131</v>
+      </c>
+      <c r="C18">
+        <v>0.30945990000000001</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1.6186999999999999E-4</v>
+        <v>147</v>
+      </c>
+      <c r="C19">
+        <v>0.29207715000000001</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.6147000000000001E-4</v>
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>0.28233412000000002</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
-        <v>62</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1.3187999999999999E-4</v>
+        <v>186</v>
+      </c>
+      <c r="C21">
+        <v>0.26683760000000001</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1.0333E-4</v>
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>0.26538157000000001</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -2095,41 +2105,41 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1.0013000000000001E-4</v>
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <v>0.22609465000000001</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="1">
-        <v>7.8200000000000003E-5</v>
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>0.18956655</v>
       </c>
       <c r="D24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="1">
-        <v>7.6320000000000001E-5</v>
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>0.15321626999999999</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -2137,55 +2147,55 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
-        <v>67</v>
+        <v>183</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="1">
-        <v>7.0759999999999993E-5</v>
+        <v>185</v>
+      </c>
+      <c r="C26">
+        <v>0.10608434999999999</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="1">
-        <v>6.6710000000000003E-5</v>
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>0.10593935</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="1">
-        <v>5.4610000000000001E-5</v>
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>9.5289070000000003E-2</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="1">
-        <v>5.2490000000000001E-5</v>
+        <v>183</v>
+      </c>
+      <c r="C29">
+        <v>9.3178789999999997E-2</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -2193,13 +2203,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5.117E-5</v>
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>3.4280399999999998E-3</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2207,13 +2217,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="1">
-        <v>4.706E-5</v>
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>2.8281399999999998E-3</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -2221,69 +2231,69 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
-      </c>
-      <c r="C32" s="1">
-        <v>4.07E-5</v>
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>1.3479900000000001E-3</v>
       </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="5">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="1">
-        <v>3.561E-5</v>
+        <v>52</v>
+      </c>
+      <c r="C33">
+        <v>1.3235499999999999E-3</v>
       </c>
       <c r="D33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3.252E-5</v>
+        <v>51</v>
+      </c>
+      <c r="C34">
+        <v>1.19169E-3</v>
       </c>
       <c r="D34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2.472E-5</v>
+        <v>72</v>
+      </c>
+      <c r="C35">
+        <v>7.6369000000000003E-4</v>
       </c>
       <c r="D35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="1">
-        <v>2.37E-5</v>
+        <v>91</v>
+      </c>
+      <c r="C36">
+        <v>7.6256000000000002E-4</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -2291,13 +2301,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2.071E-5</v>
+        <v>63</v>
+      </c>
+      <c r="C37">
+        <v>4.9850000000000003E-4</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -2305,27 +2315,27 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1.821E-5</v>
+        <v>46</v>
+      </c>
+      <c r="C38">
+        <v>3.0278999999999999E-4</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1.7249999999999999E-5</v>
+        <v>44</v>
+      </c>
+      <c r="C39">
+        <v>1.8016000000000001E-4</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -2333,13 +2343,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1.378E-5</v>
+        <v>87</v>
+      </c>
+      <c r="C40">
+        <v>1.6593000000000001E-4</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -2347,13 +2357,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1.36E-5</v>
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>1.6186999999999999E-4</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -2361,13 +2371,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1.2999999999999999E-5</v>
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>1.6147000000000001E-4</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -2375,13 +2385,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1.2799999999999999E-5</v>
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>1.0013000000000001E-4</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -2389,27 +2399,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1.15E-5</v>
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>7.8200000000000003E-5</v>
       </c>
       <c r="D44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1.045E-5</v>
+        <v>69</v>
+      </c>
+      <c r="C45">
+        <v>7.0759999999999993E-5</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2417,13 +2427,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="1">
-        <v>9.4299999999999995E-6</v>
+        <v>90</v>
+      </c>
+      <c r="C46">
+        <v>6.6710000000000003E-5</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2431,13 +2441,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="1">
-        <v>9.02E-6</v>
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <v>5.4610000000000001E-5</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -2445,27 +2455,27 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="1">
-        <v>8.3000000000000002E-6</v>
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>5.414E-5</v>
       </c>
       <c r="D48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="1">
-        <v>7.3900000000000004E-6</v>
+        <v>24</v>
+      </c>
+      <c r="C49">
+        <v>5.1900000000000001E-5</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -2473,41 +2483,41 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="1">
-        <v>6.6800000000000004E-6</v>
+        <v>62</v>
+      </c>
+      <c r="C50">
+        <v>5.117E-5</v>
       </c>
       <c r="D50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="1">
-        <v>5.3299999999999998E-6</v>
+        <v>89</v>
+      </c>
+      <c r="C51">
+        <v>4.706E-5</v>
       </c>
       <c r="D51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="1">
-        <v>4.5700000000000003E-6</v>
+        <v>64</v>
+      </c>
+      <c r="C52">
+        <v>4.4889999999999999E-5</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -2515,13 +2525,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="1">
-        <v>4.5399999999999997E-6</v>
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>3.6560000000000002E-5</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -2529,41 +2539,41 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
-      </c>
-      <c r="C54" s="1">
-        <v>4.33E-6</v>
+        <v>65</v>
+      </c>
+      <c r="C54">
+        <v>2.37E-5</v>
       </c>
       <c r="D54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
-      </c>
-      <c r="C55" s="1">
-        <v>4.1699999999999999E-6</v>
+        <v>78</v>
+      </c>
+      <c r="C55">
+        <v>2.071E-5</v>
       </c>
       <c r="D55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="1">
-        <v>4.1200000000000004E-6</v>
+        <v>88</v>
+      </c>
+      <c r="C56">
+        <v>1.7249999999999999E-5</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -2571,27 +2581,27 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="1">
-        <v>3.4300000000000002E-6</v>
+        <v>48</v>
+      </c>
+      <c r="C57">
+        <v>1.378E-5</v>
       </c>
       <c r="D57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="1">
-        <v>2.7099999999999999E-6</v>
+        <v>86</v>
+      </c>
+      <c r="C58">
+        <v>1.36E-5</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -2599,55 +2609,55 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
-        <v>185</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
-      </c>
-      <c r="C59" s="1">
-        <v>2.4499999999999998E-6</v>
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>1.2999999999999999E-5</v>
       </c>
       <c r="D59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
-      </c>
-      <c r="C60" s="1">
-        <v>1.9199999999999998E-6</v>
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>1.287E-5</v>
       </c>
       <c r="D60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1.3400000000000001E-6</v>
+        <v>77</v>
+      </c>
+      <c r="C61">
+        <v>1.2799999999999999E-5</v>
       </c>
       <c r="D61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1.28E-6</v>
+        <v>83</v>
+      </c>
+      <c r="C62">
+        <v>1.045E-5</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -2655,13 +2665,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1.15E-6</v>
+        <v>67</v>
+      </c>
+      <c r="C63">
+        <v>9.4299999999999995E-6</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -2669,41 +2679,41 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1.15E-6</v>
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <v>9.02E-6</v>
       </c>
       <c r="D64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
         <v>10</v>
       </c>
-      <c r="B65" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1.02E-6</v>
+      <c r="C65">
+        <v>7.3900000000000004E-6</v>
       </c>
       <c r="D65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" s="1">
-        <v>8.7000000000000003E-7</v>
+        <v>19</v>
+      </c>
+      <c r="C66">
+        <v>4.5700000000000003E-6</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -2711,13 +2721,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" s="1">
-        <v>8.2999999999999999E-7</v>
+        <v>81</v>
+      </c>
+      <c r="C67">
+        <v>4.5399999999999997E-6</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -2725,13 +2735,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
-      </c>
-      <c r="C68" s="1">
-        <v>6.4000000000000001E-7</v>
+        <v>31</v>
+      </c>
+      <c r="C68">
+        <v>4.1200000000000004E-6</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -2739,13 +2749,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" s="1">
-        <v>5.3000000000000001E-7</v>
+        <v>54</v>
+      </c>
+      <c r="C69">
+        <v>3.2899999999999998E-6</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -2753,13 +2763,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="1">
-        <v>4.4000000000000002E-7</v>
+        <v>76</v>
+      </c>
+      <c r="C70">
+        <v>2.7099999999999999E-6</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -2767,13 +2777,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" s="1">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="C71">
+        <v>1.28E-6</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -2781,27 +2791,27 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="5">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" s="1">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="C72">
+        <v>1.15E-6</v>
       </c>
       <c r="D72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="5">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="1">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="C73">
+        <v>8.7000000000000003E-7</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -2809,13 +2819,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="5">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" s="1">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="C74">
+        <v>8.2999999999999999E-7</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -2823,13 +2833,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="5">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
-      </c>
-      <c r="C75" s="1">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C75">
+        <v>6.4000000000000001E-7</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -2837,12 +2847,12 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>14</v>
-      </c>
-      <c r="C76" s="1">
+        <v>3</v>
+      </c>
+      <c r="C76">
         <v>0</v>
       </c>
       <c r="D76" t="b">
@@ -2851,12 +2861,12 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="5">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
-      </c>
-      <c r="C77" s="1">
+        <v>6</v>
+      </c>
+      <c r="C77">
         <v>0</v>
       </c>
       <c r="D77" t="b">
@@ -2865,12 +2875,12 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="5">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
-      </c>
-      <c r="C78" s="1">
+        <v>9</v>
+      </c>
+      <c r="C78">
         <v>0</v>
       </c>
       <c r="D78" t="b">
@@ -2879,12 +2889,12 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="5">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
-      </c>
-      <c r="C79" s="1">
+        <v>13</v>
+      </c>
+      <c r="C79">
         <v>0</v>
       </c>
       <c r="D79" t="b">
@@ -2893,26 +2903,26 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="5">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="1">
+        <v>14</v>
+      </c>
+      <c r="C80">
         <v>0</v>
       </c>
       <c r="D80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="5">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B81" t="s">
-        <v>27</v>
-      </c>
-      <c r="C81" s="1">
+        <v>17</v>
+      </c>
+      <c r="C81">
         <v>0</v>
       </c>
       <c r="D81" t="b">
@@ -2921,12 +2931,12 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="5">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>29</v>
-      </c>
-      <c r="C82" s="1">
+        <v>18</v>
+      </c>
+      <c r="C82">
         <v>0</v>
       </c>
       <c r="D82" t="b">
@@ -2935,12 +2945,12 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="5">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>30</v>
-      </c>
-      <c r="C83" s="1">
+        <v>21</v>
+      </c>
+      <c r="C83">
         <v>0</v>
       </c>
       <c r="D83" t="b">
@@ -2949,12 +2959,12 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="5">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>34</v>
-      </c>
-      <c r="C84" s="1">
+        <v>27</v>
+      </c>
+      <c r="C84">
         <v>0</v>
       </c>
       <c r="D84" t="b">
@@ -2963,12 +2973,12 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="5">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
-      </c>
-      <c r="C85" s="1">
+        <v>29</v>
+      </c>
+      <c r="C85">
         <v>0</v>
       </c>
       <c r="D85" t="b">
@@ -2977,12 +2987,12 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="5">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>47</v>
-      </c>
-      <c r="C86" s="1">
+        <v>30</v>
+      </c>
+      <c r="C86">
         <v>0</v>
       </c>
       <c r="D86" t="b">
@@ -2991,12 +3001,12 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="5">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
-      </c>
-      <c r="C87" s="1">
+        <v>34</v>
+      </c>
+      <c r="C87">
         <v>0</v>
       </c>
       <c r="D87" t="b">
@@ -3005,12 +3015,12 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="5">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
-      </c>
-      <c r="C88" s="1">
+        <v>41</v>
+      </c>
+      <c r="C88">
         <v>0</v>
       </c>
       <c r="D88" t="b">
@@ -3019,12 +3029,12 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="5">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
-        <v>55</v>
-      </c>
-      <c r="C89" s="1">
+        <v>47</v>
+      </c>
+      <c r="C89">
         <v>0</v>
       </c>
       <c r="D89" t="b">
@@ -3033,12 +3043,12 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="5">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B90" t="s">
-        <v>57</v>
-      </c>
-      <c r="C90" s="1">
+        <v>53</v>
+      </c>
+      <c r="C90">
         <v>0</v>
       </c>
       <c r="D90" t="b">
@@ -3047,12 +3057,12 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="5">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B91" t="s">
-        <v>59</v>
-      </c>
-      <c r="C91" s="1">
+        <v>55</v>
+      </c>
+      <c r="C91">
         <v>0</v>
       </c>
       <c r="D91" t="b">
@@ -3061,12 +3071,12 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="5">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B92" t="s">
-        <v>61</v>
-      </c>
-      <c r="C92" s="1">
+        <v>57</v>
+      </c>
+      <c r="C92">
         <v>0</v>
       </c>
       <c r="D92" t="b">
@@ -3075,12 +3085,12 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="5">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>68</v>
-      </c>
-      <c r="C93" s="1">
+        <v>59</v>
+      </c>
+      <c r="C93">
         <v>0</v>
       </c>
       <c r="D93" t="b">
@@ -3089,12 +3099,12 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="5">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B94" t="s">
-        <v>70</v>
-      </c>
-      <c r="C94" s="1">
+        <v>61</v>
+      </c>
+      <c r="C94">
         <v>0</v>
       </c>
       <c r="D94" t="b">
@@ -3103,12 +3113,12 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="5">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B95" t="s">
-        <v>71</v>
-      </c>
-      <c r="C95" s="1">
+        <v>68</v>
+      </c>
+      <c r="C95">
         <v>0</v>
       </c>
       <c r="D95" t="b">
@@ -3117,12 +3127,12 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="5">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B96" t="s">
-        <v>73</v>
-      </c>
-      <c r="C96" s="1">
+        <v>70</v>
+      </c>
+      <c r="C96">
         <v>0</v>
       </c>
       <c r="D96" t="b">
@@ -3131,12 +3141,12 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="5">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B97" t="s">
-        <v>75</v>
-      </c>
-      <c r="C97" s="1">
+        <v>71</v>
+      </c>
+      <c r="C97">
         <v>0</v>
       </c>
       <c r="D97" t="b">
@@ -3145,12 +3155,12 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="5">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B98" t="s">
-        <v>79</v>
-      </c>
-      <c r="C98" s="1">
+        <v>73</v>
+      </c>
+      <c r="C98">
         <v>0</v>
       </c>
       <c r="D98" t="b">
@@ -3159,12 +3169,12 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="5">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B99" t="s">
-        <v>80</v>
-      </c>
-      <c r="C99" s="1">
+        <v>75</v>
+      </c>
+      <c r="C99">
         <v>0</v>
       </c>
       <c r="D99" t="b">
@@ -3173,12 +3183,12 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="5">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B100" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="1">
+        <v>79</v>
+      </c>
+      <c r="C100">
         <v>0</v>
       </c>
       <c r="D100" t="b">
@@ -3187,12 +3197,12 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="5">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
-      </c>
-      <c r="C101" s="1">
+        <v>80</v>
+      </c>
+      <c r="C101">
         <v>0</v>
       </c>
       <c r="D101" t="b">
@@ -3201,12 +3211,12 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="5">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
-      </c>
-      <c r="C102" s="1">
+        <v>82</v>
+      </c>
+      <c r="C102">
         <v>0</v>
       </c>
       <c r="D102" t="b">
@@ -3215,12 +3225,12 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="5">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B103" t="s">
-        <v>92</v>
-      </c>
-      <c r="C103" s="1">
+        <v>84</v>
+      </c>
+      <c r="C103">
         <v>0</v>
       </c>
       <c r="D103" t="b">
@@ -3229,12 +3239,12 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="5">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B104" t="s">
-        <v>93</v>
-      </c>
-      <c r="C104" s="1">
+        <v>85</v>
+      </c>
+      <c r="C104">
         <v>0</v>
       </c>
       <c r="D104" t="b">
@@ -3243,26 +3253,26 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="5">
+        <v>90</v>
+      </c>
+      <c r="B105" t="s">
         <v>92</v>
       </c>
-      <c r="B105" t="s">
-        <v>94</v>
-      </c>
-      <c r="C105" s="1">
+      <c r="C105">
         <v>0</v>
       </c>
       <c r="D105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="5">
+        <v>91</v>
+      </c>
+      <c r="B106" t="s">
         <v>93</v>
       </c>
-      <c r="B106" t="s">
-        <v>95</v>
-      </c>
-      <c r="C106" s="1">
+      <c r="C106">
         <v>0</v>
       </c>
       <c r="D106" t="b">
@@ -3271,12 +3281,12 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="5">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>96</v>
-      </c>
-      <c r="C107" s="1">
+        <v>95</v>
+      </c>
+      <c r="C107">
         <v>0</v>
       </c>
       <c r="D107" t="b">
@@ -3285,12 +3295,12 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="5">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>97</v>
-      </c>
-      <c r="C108" s="1">
+        <v>96</v>
+      </c>
+      <c r="C108">
         <v>0</v>
       </c>
       <c r="D108" t="b">
@@ -3299,12 +3309,12 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" s="5">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B109" t="s">
-        <v>98</v>
-      </c>
-      <c r="C109" s="1">
+        <v>97</v>
+      </c>
+      <c r="C109">
         <v>0</v>
       </c>
       <c r="D109" t="b">
@@ -3313,12 +3323,12 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" s="5">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B110" t="s">
-        <v>99</v>
-      </c>
-      <c r="C110" s="1">
+        <v>98</v>
+      </c>
+      <c r="C110">
         <v>0</v>
       </c>
       <c r="D110" t="b">
@@ -3327,12 +3337,12 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" s="5">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
-      </c>
-      <c r="C111" s="1">
+        <v>99</v>
+      </c>
+      <c r="C111">
         <v>0</v>
       </c>
       <c r="D111" t="b">
@@ -3341,12 +3351,12 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112" s="5">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
-      </c>
-      <c r="C112" s="1">
+        <v>100</v>
+      </c>
+      <c r="C112">
         <v>0</v>
       </c>
       <c r="D112" t="b">
@@ -3355,12 +3365,12 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" s="5">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>102</v>
-      </c>
-      <c r="C113" s="1">
+        <v>101</v>
+      </c>
+      <c r="C113">
         <v>0</v>
       </c>
       <c r="D113" t="b">
@@ -3369,12 +3379,12 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114" s="5">
+        <v>100</v>
+      </c>
+      <c r="B114" t="s">
         <v>102</v>
       </c>
-      <c r="B114" t="s">
-        <v>104</v>
-      </c>
-      <c r="C114" s="1">
+      <c r="C114">
         <v>0</v>
       </c>
       <c r="D114" t="b">
@@ -3383,12 +3393,12 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115" s="5">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B115" t="s">
-        <v>105</v>
-      </c>
-      <c r="C115" s="1">
+        <v>104</v>
+      </c>
+      <c r="C115">
         <v>0</v>
       </c>
       <c r="D115" t="b">
@@ -3397,12 +3407,12 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" s="5">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B116" t="s">
-        <v>106</v>
-      </c>
-      <c r="C116" s="1">
+        <v>105</v>
+      </c>
+      <c r="C116">
         <v>0</v>
       </c>
       <c r="D116" t="b">
@@ -3411,12 +3421,12 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117" s="5">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B117" t="s">
-        <v>107</v>
-      </c>
-      <c r="C117" s="1">
+        <v>106</v>
+      </c>
+      <c r="C117">
         <v>0</v>
       </c>
       <c r="D117" t="b">
@@ -3425,12 +3435,12 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118" s="5">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B118" t="s">
-        <v>108</v>
-      </c>
-      <c r="C118" s="1">
+        <v>107</v>
+      </c>
+      <c r="C118">
         <v>0</v>
       </c>
       <c r="D118" t="b">
@@ -3439,12 +3449,12 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" s="5">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B119" t="s">
-        <v>109</v>
-      </c>
-      <c r="C119" s="1">
+        <v>108</v>
+      </c>
+      <c r="C119">
         <v>0</v>
       </c>
       <c r="D119" t="b">
@@ -3453,12 +3463,12 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120" s="5">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B120" t="s">
-        <v>110</v>
-      </c>
-      <c r="C120" s="1">
+        <v>109</v>
+      </c>
+      <c r="C120">
         <v>0</v>
       </c>
       <c r="D120" t="b">
@@ -3467,12 +3477,12 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121" s="5">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B121" t="s">
-        <v>111</v>
-      </c>
-      <c r="C121" s="1">
+        <v>110</v>
+      </c>
+      <c r="C121">
         <v>0</v>
       </c>
       <c r="D121" t="b">
@@ -3481,12 +3491,12 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122" s="5">
+        <v>109</v>
+      </c>
+      <c r="B122" t="s">
         <v>111</v>
       </c>
-      <c r="B122" t="s">
-        <v>113</v>
-      </c>
-      <c r="C122" s="1">
+      <c r="C122">
         <v>0</v>
       </c>
       <c r="D122" t="b">
@@ -3495,12 +3505,12 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123" s="5">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
-      </c>
-      <c r="C123" s="1">
+        <v>113</v>
+      </c>
+      <c r="C123">
         <v>0</v>
       </c>
       <c r="D123" t="b">
@@ -3509,12 +3519,12 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124" s="5">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
-      </c>
-      <c r="C124" s="1">
+        <v>114</v>
+      </c>
+      <c r="C124">
         <v>0</v>
       </c>
       <c r="D124" t="b">
@@ -3523,12 +3533,12 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125" s="5">
+        <v>113</v>
+      </c>
+      <c r="B125" t="s">
         <v>115</v>
       </c>
-      <c r="B125" t="s">
-        <v>117</v>
-      </c>
-      <c r="C125" s="1">
+      <c r="C125">
         <v>0</v>
       </c>
       <c r="D125" t="b">
@@ -3537,12 +3547,12 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126" s="5">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B126" t="s">
-        <v>118</v>
-      </c>
-      <c r="C126" s="1">
+        <v>117</v>
+      </c>
+      <c r="C126">
         <v>0</v>
       </c>
       <c r="D126" t="b">
@@ -3551,12 +3561,12 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127" s="5">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B127" t="s">
-        <v>119</v>
-      </c>
-      <c r="C127" s="1">
+        <v>118</v>
+      </c>
+      <c r="C127">
         <v>0</v>
       </c>
       <c r="D127" t="b">
@@ -3565,12 +3575,12 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" s="5">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B128" t="s">
-        <v>120</v>
-      </c>
-      <c r="C128" s="1">
+        <v>119</v>
+      </c>
+      <c r="C128">
         <v>0</v>
       </c>
       <c r="D128" t="b">
@@ -3579,16 +3589,16 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129" s="5">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B129" t="s">
-        <v>121</v>
-      </c>
-      <c r="C129" s="1">
+        <v>120</v>
+      </c>
+      <c r="C129">
         <v>0</v>
       </c>
       <c r="D129" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.45">
@@ -3598,7 +3608,7 @@
       <c r="B130" t="s">
         <v>122</v>
       </c>
-      <c r="C130" s="1">
+      <c r="C130">
         <v>0</v>
       </c>
       <c r="D130" t="b">
@@ -3612,7 +3622,7 @@
       <c r="B131" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131">
         <v>0</v>
       </c>
       <c r="D131" t="b">
@@ -3626,7 +3636,7 @@
       <c r="B132" t="s">
         <v>124</v>
       </c>
-      <c r="C132" s="1">
+      <c r="C132">
         <v>0</v>
       </c>
       <c r="D132" t="b">
@@ -3640,7 +3650,7 @@
       <c r="B133" t="s">
         <v>125</v>
       </c>
-      <c r="C133" s="1">
+      <c r="C133">
         <v>0</v>
       </c>
       <c r="D133" t="b">
@@ -3654,7 +3664,7 @@
       <c r="B134" t="s">
         <v>127</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134">
         <v>0</v>
       </c>
       <c r="D134" t="b">
@@ -3668,7 +3678,7 @@
       <c r="B135" t="s">
         <v>128</v>
       </c>
-      <c r="C135" s="1">
+      <c r="C135">
         <v>0</v>
       </c>
       <c r="D135" t="b">
@@ -3682,7 +3692,7 @@
       <c r="B136" t="s">
         <v>129</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136">
         <v>0</v>
       </c>
       <c r="D136" t="b">
@@ -3696,7 +3706,7 @@
       <c r="B137" t="s">
         <v>130</v>
       </c>
-      <c r="C137" s="1">
+      <c r="C137">
         <v>0</v>
       </c>
       <c r="D137" t="b">
@@ -3710,7 +3720,7 @@
       <c r="B138" t="s">
         <v>132</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C138">
         <v>0</v>
       </c>
       <c r="D138" t="b">
@@ -3724,7 +3734,7 @@
       <c r="B139" t="s">
         <v>133</v>
       </c>
-      <c r="C139" s="1">
+      <c r="C139">
         <v>0</v>
       </c>
       <c r="D139" t="b">
@@ -3738,7 +3748,7 @@
       <c r="B140" t="s">
         <v>134</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140">
         <v>0</v>
       </c>
       <c r="D140" t="b">
@@ -3752,7 +3762,7 @@
       <c r="B141" t="s">
         <v>135</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C141">
         <v>0</v>
       </c>
       <c r="D141" t="b">
@@ -3766,7 +3776,7 @@
       <c r="B142" t="s">
         <v>136</v>
       </c>
-      <c r="C142" s="1">
+      <c r="C142">
         <v>0</v>
       </c>
       <c r="D142" t="b">
@@ -3780,7 +3790,7 @@
       <c r="B143" t="s">
         <v>137</v>
       </c>
-      <c r="C143" s="1">
+      <c r="C143">
         <v>0</v>
       </c>
       <c r="D143" t="b">
@@ -3794,7 +3804,7 @@
       <c r="B144" t="s">
         <v>138</v>
       </c>
-      <c r="C144" s="1">
+      <c r="C144">
         <v>0</v>
       </c>
       <c r="D144" t="b">
@@ -3808,7 +3818,7 @@
       <c r="B145" t="s">
         <v>139</v>
       </c>
-      <c r="C145" s="1">
+      <c r="C145">
         <v>0</v>
       </c>
       <c r="D145" t="b">
@@ -3822,7 +3832,7 @@
       <c r="B146" t="s">
         <v>140</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C146">
         <v>0</v>
       </c>
       <c r="D146" t="b">
@@ -3836,7 +3846,7 @@
       <c r="B147" t="s">
         <v>141</v>
       </c>
-      <c r="C147" s="1">
+      <c r="C147">
         <v>0</v>
       </c>
       <c r="D147" t="b">
@@ -3850,7 +3860,7 @@
       <c r="B148" t="s">
         <v>142</v>
       </c>
-      <c r="C148" s="1">
+      <c r="C148">
         <v>0</v>
       </c>
       <c r="D148" t="b">
@@ -3864,7 +3874,7 @@
       <c r="B149" t="s">
         <v>143</v>
       </c>
-      <c r="C149" s="1">
+      <c r="C149">
         <v>0</v>
       </c>
       <c r="D149" t="b">
@@ -3878,7 +3888,7 @@
       <c r="B150" t="s">
         <v>144</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150">
         <v>0</v>
       </c>
       <c r="D150" t="b">
@@ -3892,7 +3902,7 @@
       <c r="B151" t="s">
         <v>145</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151">
         <v>0</v>
       </c>
       <c r="D151" t="b">
@@ -3906,7 +3916,7 @@
       <c r="B152" t="s">
         <v>146</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152">
         <v>0</v>
       </c>
       <c r="D152" t="b">
@@ -3920,7 +3930,7 @@
       <c r="B153" t="s">
         <v>148</v>
       </c>
-      <c r="C153" s="1">
+      <c r="C153">
         <v>0</v>
       </c>
       <c r="D153" t="b">
@@ -3934,7 +3944,7 @@
       <c r="B154" t="s">
         <v>149</v>
       </c>
-      <c r="C154" s="1">
+      <c r="C154">
         <v>0</v>
       </c>
       <c r="D154" t="b">
@@ -3948,7 +3958,7 @@
       <c r="B155" t="s">
         <v>150</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155">
         <v>0</v>
       </c>
       <c r="D155" t="b">
@@ -3962,7 +3972,7 @@
       <c r="B156" t="s">
         <v>151</v>
       </c>
-      <c r="C156" s="1">
+      <c r="C156">
         <v>0</v>
       </c>
       <c r="D156" t="b">
@@ -3976,7 +3986,7 @@
       <c r="B157" t="s">
         <v>152</v>
       </c>
-      <c r="C157" s="1">
+      <c r="C157">
         <v>0</v>
       </c>
       <c r="D157" t="b">
@@ -3990,7 +4000,7 @@
       <c r="B158" t="s">
         <v>153</v>
       </c>
-      <c r="C158" s="1">
+      <c r="C158">
         <v>0</v>
       </c>
       <c r="D158" t="b">
@@ -4004,7 +4014,7 @@
       <c r="B159" t="s">
         <v>154</v>
       </c>
-      <c r="C159" s="1">
+      <c r="C159">
         <v>0</v>
       </c>
       <c r="D159" t="b">
@@ -4018,7 +4028,7 @@
       <c r="B160" t="s">
         <v>155</v>
       </c>
-      <c r="C160" s="1">
+      <c r="C160">
         <v>0</v>
       </c>
       <c r="D160" t="b">
@@ -4032,7 +4042,7 @@
       <c r="B161" t="s">
         <v>156</v>
       </c>
-      <c r="C161" s="1">
+      <c r="C161">
         <v>0</v>
       </c>
       <c r="D161" t="b">
@@ -4046,7 +4056,7 @@
       <c r="B162" t="s">
         <v>158</v>
       </c>
-      <c r="C162" s="1">
+      <c r="C162">
         <v>0</v>
       </c>
       <c r="D162" t="b">
@@ -4060,7 +4070,7 @@
       <c r="B163" t="s">
         <v>159</v>
       </c>
-      <c r="C163" s="1">
+      <c r="C163">
         <v>0</v>
       </c>
       <c r="D163" t="b">
@@ -4074,7 +4084,7 @@
       <c r="B164" t="s">
         <v>160</v>
       </c>
-      <c r="C164" s="1">
+      <c r="C164">
         <v>0</v>
       </c>
       <c r="D164" t="b">
@@ -4088,7 +4098,7 @@
       <c r="B165" t="s">
         <v>161</v>
       </c>
-      <c r="C165" s="1">
+      <c r="C165">
         <v>0</v>
       </c>
       <c r="D165" t="b">
@@ -4102,7 +4112,7 @@
       <c r="B166" t="s">
         <v>162</v>
       </c>
-      <c r="C166" s="1">
+      <c r="C166">
         <v>0</v>
       </c>
       <c r="D166" t="b">
@@ -4116,7 +4126,7 @@
       <c r="B167" t="s">
         <v>163</v>
       </c>
-      <c r="C167" s="1">
+      <c r="C167">
         <v>0</v>
       </c>
       <c r="D167" t="b">
@@ -4130,7 +4140,7 @@
       <c r="B168" t="s">
         <v>164</v>
       </c>
-      <c r="C168" s="1">
+      <c r="C168">
         <v>0</v>
       </c>
       <c r="D168" t="b">
@@ -4144,7 +4154,7 @@
       <c r="B169" t="s">
         <v>165</v>
       </c>
-      <c r="C169" s="1">
+      <c r="C169">
         <v>0</v>
       </c>
       <c r="D169" t="b">
@@ -4158,7 +4168,7 @@
       <c r="B170" t="s">
         <v>166</v>
       </c>
-      <c r="C170" s="1">
+      <c r="C170">
         <v>0</v>
       </c>
       <c r="D170" t="b">
@@ -4172,7 +4182,7 @@
       <c r="B171" t="s">
         <v>167</v>
       </c>
-      <c r="C171" s="1">
+      <c r="C171">
         <v>0</v>
       </c>
       <c r="D171" t="b">
@@ -4186,7 +4196,7 @@
       <c r="B172" t="s">
         <v>168</v>
       </c>
-      <c r="C172" s="1">
+      <c r="C172">
         <v>0</v>
       </c>
       <c r="D172" t="b">
@@ -4200,7 +4210,7 @@
       <c r="B173" t="s">
         <v>169</v>
       </c>
-      <c r="C173" s="1">
+      <c r="C173">
         <v>0</v>
       </c>
       <c r="D173" t="b">
@@ -4214,7 +4224,7 @@
       <c r="B174" t="s">
         <v>170</v>
       </c>
-      <c r="C174" s="1">
+      <c r="C174">
         <v>0</v>
       </c>
       <c r="D174" t="b">
@@ -4228,7 +4238,7 @@
       <c r="B175" t="s">
         <v>171</v>
       </c>
-      <c r="C175" s="1">
+      <c r="C175">
         <v>0</v>
       </c>
       <c r="D175" t="b">
@@ -4242,7 +4252,7 @@
       <c r="B176" t="s">
         <v>172</v>
       </c>
-      <c r="C176" s="1">
+      <c r="C176">
         <v>0</v>
       </c>
       <c r="D176" t="b">
@@ -4256,7 +4266,7 @@
       <c r="B177" t="s">
         <v>173</v>
       </c>
-      <c r="C177" s="1">
+      <c r="C177">
         <v>0</v>
       </c>
       <c r="D177" t="b">
@@ -4270,7 +4280,7 @@
       <c r="B178" t="s">
         <v>174</v>
       </c>
-      <c r="C178" s="1">
+      <c r="C178">
         <v>0</v>
       </c>
       <c r="D178" t="b">
@@ -4284,7 +4294,7 @@
       <c r="B179" t="s">
         <v>175</v>
       </c>
-      <c r="C179" s="1">
+      <c r="C179">
         <v>0</v>
       </c>
       <c r="D179" t="b">
@@ -4298,7 +4308,7 @@
       <c r="B180" t="s">
         <v>176</v>
       </c>
-      <c r="C180" s="1">
+      <c r="C180">
         <v>0</v>
       </c>
       <c r="D180" t="b">
@@ -4312,7 +4322,7 @@
       <c r="B181" t="s">
         <v>177</v>
       </c>
-      <c r="C181" s="1">
+      <c r="C181">
         <v>0</v>
       </c>
       <c r="D181" t="b">
@@ -4326,7 +4336,7 @@
       <c r="B182" t="s">
         <v>178</v>
       </c>
-      <c r="C182" s="1">
+      <c r="C182">
         <v>0</v>
       </c>
       <c r="D182" t="b">
@@ -4340,7 +4350,7 @@
       <c r="B183" t="s">
         <v>179</v>
       </c>
-      <c r="C183" s="1">
+      <c r="C183">
         <v>0</v>
       </c>
       <c r="D183" t="b">
@@ -4354,7 +4364,7 @@
       <c r="B184" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="1">
+      <c r="C184">
         <v>0</v>
       </c>
       <c r="D184" t="b">
@@ -4368,7 +4378,7 @@
       <c r="B185" t="s">
         <v>181</v>
       </c>
-      <c r="C185" s="1">
+      <c r="C185">
         <v>0</v>
       </c>
       <c r="D185" t="b">
@@ -4382,7 +4392,7 @@
       <c r="B186" t="s">
         <v>182</v>
       </c>
-      <c r="C186" s="1">
+      <c r="C186">
         <v>0</v>
       </c>
       <c r="D186" t="b">
@@ -4396,7 +4406,7 @@
       <c r="B187" t="s">
         <v>184</v>
       </c>
-      <c r="C187" s="1">
+      <c r="C187">
         <v>0</v>
       </c>
       <c r="D187" t="b">
@@ -4410,7 +4420,7 @@
       <c r="B188" t="s">
         <v>188</v>
       </c>
-      <c r="C188" s="1">
+      <c r="C188">
         <v>0</v>
       </c>
       <c r="D188" t="b">
@@ -4424,7 +4434,7 @@
       <c r="B189" t="s">
         <v>189</v>
       </c>
-      <c r="C189" s="1">
+      <c r="C189">
         <v>0</v>
       </c>
       <c r="D189" t="b">
@@ -4438,7 +4448,7 @@
       <c r="B190" t="s">
         <v>190</v>
       </c>
-      <c r="C190" s="1">
+      <c r="C190">
         <v>0</v>
       </c>
       <c r="D190" t="b">
@@ -4452,7 +4462,7 @@
       <c r="B191" t="s">
         <v>191</v>
       </c>
-      <c r="C191" s="1">
+      <c r="C191">
         <v>0</v>
       </c>
       <c r="D191" t="b">
@@ -4466,7 +4476,7 @@
       <c r="B192" t="s">
         <v>192</v>
       </c>
-      <c r="C192" s="1">
+      <c r="C192">
         <v>0</v>
       </c>
       <c r="D192" t="b">
@@ -4480,7 +4490,7 @@
       <c r="B193" t="s">
         <v>193</v>
       </c>
-      <c r="C193" s="1">
+      <c r="C193">
         <v>0</v>
       </c>
       <c r="D193" t="b">
@@ -4494,7 +4504,7 @@
       <c r="B194" t="s">
         <v>194</v>
       </c>
-      <c r="C194" s="1">
+      <c r="C194">
         <v>0</v>
       </c>
       <c r="D194" t="b">
@@ -4508,7 +4518,7 @@
       <c r="B195" t="s">
         <v>195</v>
       </c>
-      <c r="C195" s="1">
+      <c r="C195">
         <v>0</v>
       </c>
       <c r="D195" t="b">
@@ -4522,7 +4532,7 @@
       <c r="B196" t="s">
         <v>196</v>
       </c>
-      <c r="C196" s="1">
+      <c r="C196">
         <v>0</v>
       </c>
       <c r="D196" t="b">
@@ -4536,7 +4546,7 @@
       <c r="B197" t="s">
         <v>197</v>
       </c>
-      <c r="C197" s="1">
+      <c r="C197">
         <v>0</v>
       </c>
       <c r="D197" t="b">
@@ -4550,7 +4560,7 @@
       <c r="B198" t="s">
         <v>198</v>
       </c>
-      <c r="C198" s="1">
+      <c r="C198">
         <v>0</v>
       </c>
       <c r="D198" t="b">
@@ -4564,7 +4574,7 @@
       <c r="B199" t="s">
         <v>199</v>
       </c>
-      <c r="C199" s="1">
+      <c r="C199">
         <v>0</v>
       </c>
       <c r="D199" t="b">
@@ -4578,7 +4588,7 @@
       <c r="B200" t="s">
         <v>200</v>
       </c>
-      <c r="C200" s="1">
+      <c r="C200">
         <v>0</v>
       </c>
       <c r="D200" t="b">
@@ -4592,7 +4602,7 @@
       <c r="B201" t="s">
         <v>201</v>
       </c>
-      <c r="C201" s="1">
+      <c r="C201">
         <v>0</v>
       </c>
       <c r="D201" t="b">

</xml_diff>